<commit_message>
Fixed bug - ipopt solver yielding a t2 bound larger than tf
</commit_message>
<xml_diff>
--- a/examples/2_circle2circle_analysis_files/analysis - circle-to-same-circle_deltaV.xlsx
+++ b/examples/2_circle2circle_analysis_files/analysis - circle-to-same-circle_deltaV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trist\Documents\Astrodynamics\Numerical Models\Impulsive Thrust\Rendezvous\Optimal Two-Impulse Rendezvous\py2iopt\examples\2_circle2circle_analysis_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FFE0CA-B075-4FEE-9B30-EF5FEC91E190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAFFA80-2220-4E4D-9FC4-A2CCA68CA7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lambert" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,10 @@
     <t>infeasible</t>
   </si>
   <si>
-    <t>Lambert</t>
+    <t>Ipopt &lt; L-BFGS-B</t>
   </si>
   <si>
-    <t>Ipopt &lt; L-BFGS-B</t>
+    <t>Phasing</t>
   </si>
 </sst>
 </file>
@@ -3359,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1E60AE-D74D-4ECC-9EED-F1B306B56408}">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K22" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3373,10 +3373,10 @@
         <v>1</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>